<commit_message>
Escaleta y manuscrito CN_08_09_CO, enviado a jhon
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion09/Escaleta_CN_08_09_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion09/Escaleta_CN_08_09_CO.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado08\guion09\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7155" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DATOS" sheetId="1" state="hidden" r:id="rId1"/>
@@ -18,12 +13,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja2!$A$1:$U$27</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="225">
   <si>
     <t>Matemáticas</t>
   </si>
@@ -284,9 +279,6 @@
     <t>Los ácidos y las bases</t>
   </si>
   <si>
-    <t>Conoce más de los ácidos</t>
-  </si>
-  <si>
     <t>Interactivo que sirve para entender qué son los ácidos, sus características y cómo reaccionan con otras sustancias</t>
   </si>
   <si>
@@ -302,9 +294,6 @@
     <t>FQ_10_07</t>
   </si>
   <si>
-    <t>Conoce más de las bases</t>
-  </si>
-  <si>
     <t>Interactivo que ayuda a entender qué son los hidróxidos, sus características y la manera en que reaccionan con otras sustancias</t>
   </si>
   <si>
@@ -321,9 +310,6 @@
   </si>
   <si>
     <t>RM_01_01_CO</t>
-  </si>
-  <si>
-    <t>Herramientas para conocer el riesgo de las sustancias</t>
   </si>
   <si>
     <t>Recurso M9B-01</t>
@@ -481,35 +467,242 @@
     <t>Conoce el nombre de algunos ácidos y bases</t>
   </si>
   <si>
-    <t>Comprende características comunes perceptibles de los ácidos completando el texto</t>
-  </si>
-  <si>
-    <t>Comprende características comunes de las bases completando el texto</t>
-  </si>
-  <si>
     <t>si</t>
   </si>
   <si>
     <t>modificado 50%</t>
   </si>
   <si>
-    <t>Actividad con pictogramas de seguridad para reconocer riesgos que representan las sustancias químicas tanto ácidas y básicas entre otras</t>
-  </si>
-  <si>
-    <t>Interactivo para ver los conceptos de ácido, base y neutralización a partir de las 3 teorías</t>
-  </si>
-  <si>
-    <t>Herramientas para reconocer la importancia de la teorías ácido- base</t>
-  </si>
-  <si>
-    <t>Crucigrama que permite relacionar los temas de las 3 teorías ácido base</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: Las teorías ácido-base</t>
   </si>
   <si>
+    <t>Interactivo para conocer qué alternativas tenemos para medir pH en una solución</t>
+  </si>
+  <si>
+    <t>Distingue entre ácidos y bases usando el concepto de pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad con animación incluida diseñada para plantear en qué se diferencian los ácidos de las bases </t>
+  </si>
+  <si>
+    <t>modificado 10%</t>
+  </si>
+  <si>
+    <t>Distingue entre ácidos y bases</t>
+  </si>
+  <si>
+    <t>Comprende las características de las soluciones reguladoras de pH completando el texto</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Actividades sobre el concepto y escala de pH</t>
+  </si>
+  <si>
+    <t>Conoce los ácidos más comunes y sus usos</t>
+  </si>
+  <si>
+    <t>Actividad que presenta los ácidos más comunes y su utilidad</t>
+  </si>
+  <si>
+    <t>Descubre las bases más comunes y sus usos</t>
+  </si>
+  <si>
+    <t>Conoce las bases más comunes y sus usos</t>
+  </si>
+  <si>
+    <t>sin modificaciones</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Los ácidos y las bases en la vida cotidiana</t>
+  </si>
+  <si>
+    <t>ampliado: 4 preguntas más</t>
+  </si>
+  <si>
+    <t>Actividad que propone realizar un experimento para determinar las propiedades de los ácidos y las bases</t>
+  </si>
+  <si>
+    <t>Competencias: preparación de un indicador ácido-base</t>
+  </si>
+  <si>
+    <t>modificado 5%</t>
+  </si>
+  <si>
+    <t>Actividad que propone realizar un experimento tipo proyecto para construir la escala de pH usando dos indicadores ácido-base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evalúa tus conocimientos sobre el tema de los ácidos y las bases </t>
+  </si>
+  <si>
+    <t>Banco de actividades: Los ácidos y las bases</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>Recursos F</t>
+  </si>
+  <si>
+    <t>Recurso F6-01</t>
+  </si>
+  <si>
+    <t>RF_01_01_CO</t>
+  </si>
+  <si>
+    <t>Recurso F6-02</t>
+  </si>
+  <si>
+    <t>Recurso F13-01</t>
+  </si>
+  <si>
+    <t>Recurso M2A-02</t>
+  </si>
+  <si>
+    <t>Recurso M2A-03</t>
+  </si>
+  <si>
+    <t>Recurso M11A-01</t>
+  </si>
+  <si>
+    <t>Recurso F13B-01</t>
+  </si>
+  <si>
+    <t>Calcula el pH de las disoluciones</t>
+  </si>
+  <si>
+    <t>modificado 100%, sólo se tomó el modelo, se crearon preguntas nuevas.</t>
+  </si>
+  <si>
+    <t>CN_08_09_CO</t>
+  </si>
+  <si>
+    <t>Qué son los ácidos y las bases</t>
+  </si>
+  <si>
+    <t>La importancia de los ácidos y las bases</t>
+  </si>
+  <si>
+    <t>Actividad que permite evaluar tus conocimientos sobre el tema de los ácidos y las bases</t>
+  </si>
+  <si>
+    <t>Recurso M4A-01</t>
+  </si>
+  <si>
+    <t>Las teorías ácido-base</t>
+  </si>
+  <si>
+    <t>La teoría de Lewis</t>
+  </si>
+  <si>
+    <t>El concepto de pH</t>
+  </si>
+  <si>
+    <t>La escala de pH</t>
+  </si>
+  <si>
+    <t>Los indicadores ácido-base</t>
+  </si>
+  <si>
+    <t>Soluciones reguladoras de pH</t>
+  </si>
+  <si>
+    <t>Recurso M4A-02</t>
+  </si>
+  <si>
+    <t>Consolidación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: Los ácidos y las bases en la vida diaria </t>
+  </si>
+  <si>
+    <t>Fin de tema</t>
+  </si>
+  <si>
+    <t>Recurso M4A-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El uso de soluciones reguladoras de pH </t>
+  </si>
+  <si>
+    <t>La medición de pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las teorías ácido-base </t>
+  </si>
+  <si>
+    <t>Las características de las bases</t>
+  </si>
+  <si>
+    <t>Las características de los ácidos</t>
+  </si>
+  <si>
+    <t>Los ácidos y las bases en la vida cotidiana</t>
+  </si>
+  <si>
+    <t>Banco de actividades del tema: Los ácidos y las bases</t>
+  </si>
+  <si>
+    <t>Conoce más acerca de las bases</t>
+  </si>
+  <si>
+    <t>Conoce más acerca de los ácidos</t>
+  </si>
+  <si>
+    <t>Comprende las características comunes perceptibles de los ácidos completando el texto</t>
+  </si>
+  <si>
+    <t>Comprende las características comunes de las bases completando el texto</t>
+  </si>
+  <si>
+    <t>Las herramientas para conocer el riesgo de las sustancias</t>
+  </si>
+  <si>
+    <t>Actividad con pictogramas de seguridad para reconocer riesgos de las sustancias químicas: ácidas y básicas, entre otras</t>
+  </si>
+  <si>
+    <t>¿Qué tantos sabes de los ácidos, bases y su importancia?</t>
+  </si>
+  <si>
+    <t>Interactivo para ver los conceptos de ácido, base y neutralización a partir de las tres teorías</t>
+  </si>
+  <si>
+    <t>Las herramientas para reconocer la importancia de las teorías ácido-base</t>
+  </si>
+  <si>
+    <t>Crucigrama que permite relacionar los temas de las tres teorías ácido-base</t>
+  </si>
+  <si>
+    <t>Actividad sobre Las teorías ácido-base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para practicar el cálculo de pH y la concentración de soluciones ácidas y básicas </t>
+  </si>
+  <si>
+    <t>Actividad acerca del concepto y la escala de pH</t>
+  </si>
+  <si>
+    <t>Actividad que sirve para conocer cuáles son las bases más comunes y para que se emplean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los ácidos y las bases como sustancias de uso común </t>
+  </si>
+  <si>
+    <t>Actividad sobre los ácidos y las bases en la vida cotidiana</t>
+  </si>
+  <si>
+    <t>Proyecto: la construcción de la escala de pH</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Actividad sobre </t>
+      <t xml:space="preserve">¿Qué tanto sabes del concepto y de la escala de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>pH</t>
     </r>
     <r>
       <rPr>
@@ -518,60 +711,21 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Las teorías ácido-base</t>
+      <t>?</t>
     </r>
   </si>
   <si>
-    <t>Interactivo para conocer qué alternativas tenemos para medir pH en una solución</t>
-  </si>
-  <si>
-    <t>Distingue entre ácidos y bases usando el concepto de pH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad con animación incluida diseñada para plantear en qué se diferencian los ácidos de las bases </t>
-  </si>
-  <si>
-    <t>modificado 10%</t>
-  </si>
-  <si>
-    <t>Distingue entre ácidos y bases</t>
-  </si>
-  <si>
-    <t>Actividad para practicar el cálculo de pH y concentración de soluciones básicas y ácidas</t>
-  </si>
-  <si>
-    <t>Comprende las características de las soluciones reguladoras de pH completando el texto</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: Actividades sobre el concepto y escala de pH</t>
-  </si>
-  <si>
-    <t>Actividad acerca del concepto de pH y escala de pH</t>
-  </si>
-  <si>
-    <t>Conoce los ácidos más comunes y sus usos</t>
-  </si>
-  <si>
-    <t>Actividad que presenta los ácidos más comunes y su utilidad</t>
-  </si>
-  <si>
-    <t>Descubre las bases más comunes y sus usos</t>
-  </si>
-  <si>
-    <t>Conoce las bases más comunes y sus usos</t>
-  </si>
-  <si>
-    <t>Actividad que sirve para conocer cuáles son las bases más comunes y para qué se emplean</t>
-  </si>
-  <si>
-    <t>sin modificaciones</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: Los ácidos y las bases en la vida cotidiana</t>
-  </si>
-  <si>
     <r>
-      <t xml:space="preserve">Actividad sobre </t>
+      <t>El cálculo de pH y la concentración de</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> H₃O+ </t>
     </r>
     <r>
       <rPr>
@@ -580,159 +734,55 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>los ácidos y las bases en la vida cotidiana</t>
+      <t>en una solución</t>
     </r>
   </si>
   <si>
-    <t>ampliado: 4 preguntas más</t>
-  </si>
-  <si>
-    <t>Competencias: preparación de un indicador ácido base</t>
-  </si>
-  <si>
-    <t>Actividad que propone realizar un experimento para determinar las propiedades de los ácidos y las bases</t>
-  </si>
-  <si>
-    <t>Competencias: preparación de un indicador ácido-base</t>
-  </si>
-  <si>
-    <t>modificado 5%</t>
-  </si>
-  <si>
-    <t>Actividad que propone realizar un experimento tipo proyecto para construir la escala de pH usando dos indicadores ácido-base</t>
-  </si>
-  <si>
-    <t>Mapa conceptual del tema Ácidos y Bases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Evalúa tus conocimientos sobre el tema de los ácidos y las bases </t>
-  </si>
-  <si>
-    <t>Banco de actividades: Los ácidos y las bases</t>
-  </si>
-  <si>
-    <t>RF</t>
-  </si>
-  <si>
-    <t>Recursos F</t>
-  </si>
-  <si>
-    <t>Recurso F6-01</t>
-  </si>
-  <si>
-    <t>RF_01_01_CO</t>
-  </si>
-  <si>
-    <t>Recurso F6-02</t>
-  </si>
-  <si>
-    <t>Recurso F13-01</t>
-  </si>
-  <si>
-    <t>Recurso M2A-02</t>
-  </si>
-  <si>
-    <t>Recurso M2A-03</t>
-  </si>
-  <si>
-    <t>Recurso M11A-01</t>
-  </si>
-  <si>
-    <t>Recurso F13B-01</t>
-  </si>
-  <si>
-    <t>Calcula el pH de las disoluciones</t>
-  </si>
-  <si>
-    <t>modificado 100%, sólo se tomó el modelo, se crearon preguntas nuevas.</t>
-  </si>
-  <si>
-    <t>CN_08_09_CO</t>
-  </si>
-  <si>
-    <t>Qué son los ácidos y las bases</t>
-  </si>
-  <si>
-    <t>La importancia de los ácidos y las bases</t>
-  </si>
-  <si>
-    <t>Actividad que permite evaluar tus conocimientos sobre el tema de los ácidos y las bases</t>
-  </si>
-  <si>
-    <t>Recurso M4A-01</t>
-  </si>
-  <si>
-    <t>Las teorías ácido-base</t>
-  </si>
-  <si>
-    <t>La teoría de Lewis</t>
-  </si>
-  <si>
-    <t>El concepto de pH</t>
-  </si>
-  <si>
-    <t>La escala de pH</t>
-  </si>
-  <si>
-    <t>Los indicadores ácido-base</t>
-  </si>
-  <si>
-    <t>El cálculo de pH y concentración en una solución</t>
-  </si>
-  <si>
-    <t>Soluciones reguladoras de pH</t>
-  </si>
-  <si>
-    <t>Actividad que permite evaluar tus conocimientos sobre eel tema de ph</t>
-  </si>
-  <si>
-    <t>Recurso M4A-02</t>
-  </si>
-  <si>
-    <t>Consolidación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: Los ácidos y las bases en la vida diaria </t>
-  </si>
-  <si>
-    <t>Fin de tema</t>
-  </si>
-  <si>
-    <t>Mapa conceptual sobre el tema: Los ácidos y las bases</t>
-  </si>
-  <si>
-    <t>Recurso M4A-03</t>
-  </si>
-  <si>
-    <t>Proyecto: construcción de la escala de pH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El uso de soluciones reguladoras de pH </t>
-  </si>
-  <si>
-    <t>La medición de pH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Las teorías ácido-base </t>
-  </si>
-  <si>
-    <t>Las características de las bases</t>
-  </si>
-  <si>
-    <t>Las características de los ácidos</t>
-  </si>
-  <si>
-    <t>Los ácidos y las bases en la vida cotidiana</t>
-  </si>
-  <si>
-    <t>Banco de actividades del tema: Los ácidos y las bases</t>
+    <r>
+      <t xml:space="preserve">Actividad que permite evaluar tus conocimientos sobre el tema de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>pH</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Competencias: preparación de un indicador ácido</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>base</t>
+    </r>
+  </si>
+  <si>
+    <t>Mapa conceptual sobre el tema Los ácidos y las bases</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -783,6 +833,17 @@
     <font>
       <sz val="12"/>
       <color rgb="FF222222"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -938,7 +999,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1169,6 +1230,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1274,7 +1338,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1309,7 +1373,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3482,10 +3546,10 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:U118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="K23" sqref="K23"/>
+      <selection pane="bottomLeft" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3495,10 +3559,10 @@
     <col min="3" max="3" width="21.140625" style="29" customWidth="1"/>
     <col min="4" max="4" width="34.140625" style="16" customWidth="1"/>
     <col min="5" max="5" width="32.85546875" style="25" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" style="26" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="40.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" style="26" customWidth="1"/>
+    <col min="7" max="7" width="55.28515625" style="5" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" style="27" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="5" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="47.7109375" style="9" customWidth="1"/>
     <col min="11" max="11" width="18.85546875" style="31" customWidth="1"/>
     <col min="12" max="12" width="21.5703125" style="31" customWidth="1"/>
@@ -3515,124 +3579,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="12" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="86" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="89" t="s">
+      <c r="D1" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="88" t="s">
+      <c r="E1" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="91" t="s">
+      <c r="F1" s="92" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="83" t="s">
+      <c r="G1" s="84" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="83" t="s">
+      <c r="H1" s="84" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="83" t="s">
+      <c r="I1" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="87" t="s">
+      <c r="J1" s="88" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="86" t="s">
+      <c r="K1" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="86" t="s">
+      <c r="L1" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="86" t="s">
+      <c r="M1" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="N1" s="86"/>
-      <c r="O1" s="80" t="s">
+      <c r="N1" s="87"/>
+      <c r="O1" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="P1" s="79" t="s">
+      <c r="P1" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="Q1" s="81" t="s">
+      <c r="Q1" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="R1" s="82" t="s">
+      <c r="R1" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="S1" s="81" t="s">
+      <c r="S1" s="82" t="s">
         <v>80</v>
       </c>
-      <c r="T1" s="82" t="s">
+      <c r="T1" s="83" t="s">
         <v>81</v>
       </c>
-      <c r="U1" s="81" t="s">
+      <c r="U1" s="82" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="12" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="85"/>
-      <c r="B2" s="84"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
+      <c r="A2" s="86"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
       <c r="M2" s="8" t="s">
         <v>83</v>
       </c>
       <c r="N2" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="81"/>
-      <c r="T2" s="82"/>
-      <c r="U2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="83"/>
+      <c r="U2" s="82"/>
     </row>
     <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>85</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
       <c r="G3" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H3" s="19">
         <v>1</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K3" s="20" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L3" s="20" t="s">
         <v>1</v>
@@ -3648,247 +3712,247 @@
         <v>6</v>
       </c>
       <c r="R3" s="34" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="S3" s="22" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="T3" s="23" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="U3" s="22" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>85</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" s="18"/>
+        <v>89</v>
+      </c>
       <c r="G4" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="H4" s="19">
+        <v>204</v>
+      </c>
+      <c r="H4" s="27">
         <v>2</v>
       </c>
       <c r="I4" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="21" t="s">
         <v>146</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="L4" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="P4" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="33">
-        <v>6</v>
+      <c r="Q4" s="33" t="s">
+        <v>87</v>
       </c>
       <c r="R4" s="34" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="S4" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="T4" s="23" t="s">
-        <v>97</v>
+        <v>85</v>
+      </c>
+      <c r="T4" s="16" t="s">
+        <v>89</v>
       </c>
       <c r="U4" s="22" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>85</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>90</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="F5" s="18"/>
       <c r="G5" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="H5" s="27">
+        <v>200</v>
+      </c>
+      <c r="H5" s="19">
         <v>3</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>87</v>
+        <v>205</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="21" t="s">
-        <v>151</v>
+      <c r="N5" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="P5" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="Q5" s="33" t="s">
-        <v>88</v>
+      <c r="Q5" s="33">
+        <v>6</v>
       </c>
       <c r="R5" s="34" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="S5" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="T5" s="16" t="s">
-        <v>90</v>
+        <v>94</v>
+      </c>
+      <c r="T5" s="23" t="s">
+        <v>95</v>
       </c>
       <c r="U5" s="22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>85</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="H6" s="19">
         <v>4</v>
       </c>
       <c r="I6" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="21" t="s">
         <v>146</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="L6" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="P6" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="Q6" s="33">
-        <v>6</v>
+      <c r="Q6" s="33" t="s">
+        <v>87</v>
       </c>
       <c r="R6" s="34" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="S6" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="T6" s="23" t="s">
-        <v>190</v>
+        <v>85</v>
+      </c>
+      <c r="T6" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="U6" s="22" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>85</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>92</v>
+        <v>199</v>
       </c>
       <c r="H7" s="19">
         <v>5</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>93</v>
+        <v>206</v>
       </c>
       <c r="K7" s="20" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="21" t="s">
-        <v>151</v>
+      <c r="N7" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="P7" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="Q7" s="33" t="s">
-        <v>88</v>
+      <c r="Q7" s="33">
+        <v>6</v>
       </c>
       <c r="R7" s="34" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="S7" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="T7" s="16" t="s">
         <v>94</v>
       </c>
+      <c r="T7" s="23" t="s">
+        <v>174</v>
+      </c>
       <c r="U7" s="22" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -3896,31 +3960,31 @@
         <v>10</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>85</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>99</v>
+        <v>207</v>
       </c>
       <c r="H8" s="27">
         <v>6</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>152</v>
+        <v>208</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L8" s="20" t="s">
         <v>14</v>
@@ -3936,16 +4000,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="S8" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="T8" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="U8" s="22" t="s">
         <v>96</v>
-      </c>
-      <c r="T8" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="U8" s="22" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3953,31 +4017,31 @@
         <v>10</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>85</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>107</v>
+        <v>209</v>
       </c>
       <c r="H9" s="19">
         <v>7</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L9" s="20" t="s">
         <v>14</v>
@@ -3993,16 +4057,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="S9" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="T9" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="U9" s="22" t="s">
         <v>96</v>
-      </c>
-      <c r="T9" s="23" t="s">
-        <v>200</v>
-      </c>
-      <c r="U9" s="22" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4010,32 +4074,32 @@
         <v>10</v>
       </c>
       <c r="B10" s="53" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C10" s="54" t="s">
         <v>85</v>
       </c>
       <c r="D10" s="55" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="E10" s="56" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="F10" s="57"/>
       <c r="G10" s="58" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H10" s="60">
         <v>8</v>
       </c>
       <c r="I10" s="60" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J10" s="68" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K10" s="62" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L10" s="62" t="s">
         <v>14</v>
@@ -4052,16 +4116,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="66" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="S10" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="T10" s="69" t="s">
+        <v>100</v>
+      </c>
+      <c r="U10" s="67" t="s">
         <v>96</v>
-      </c>
-      <c r="T10" s="69" t="s">
-        <v>103</v>
-      </c>
-      <c r="U10" s="67" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4069,30 +4133,30 @@
         <v>10</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C11" s="37" t="s">
         <v>85</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="E11" s="39"/>
       <c r="F11" s="40"/>
       <c r="G11" s="41" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="H11" s="42">
         <v>9</v>
       </c>
       <c r="I11" s="43" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="J11" s="44" t="s">
-        <v>153</v>
+        <v>210</v>
       </c>
       <c r="K11" s="45" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L11" s="45" t="s">
         <v>1</v>
@@ -4109,16 +4173,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="49" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="S11" s="50" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="T11" s="51" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="U11" s="50" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -4126,31 +4190,31 @@
         <v>10</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>85</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>154</v>
+        <v>211</v>
       </c>
       <c r="H12" s="19">
         <v>10</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="K12" s="20" t="s">
-        <v>146</v>
+        <v>212</v>
+      </c>
+      <c r="K12" s="79" t="s">
+        <v>143</v>
       </c>
       <c r="L12" s="20" t="s">
         <v>14</v>
@@ -4166,16 +4230,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="S12" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="T12" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="U12" s="22" t="s">
         <v>96</v>
-      </c>
-      <c r="T12" s="23" t="s">
-        <v>192</v>
-      </c>
-      <c r="U12" s="22" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4183,32 +4247,32 @@
         <v>10</v>
       </c>
       <c r="B13" s="53" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C13" s="54" t="s">
         <v>85</v>
       </c>
       <c r="D13" s="55" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="E13" s="56" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="F13" s="57"/>
       <c r="G13" s="58" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="H13" s="60">
         <v>11</v>
       </c>
       <c r="I13" s="60" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J13" s="68" t="s">
-        <v>157</v>
+        <v>213</v>
       </c>
       <c r="K13" s="62" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L13" s="62" t="s">
         <v>14</v>
@@ -4225,16 +4289,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="66" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="S13" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="T13" s="69" t="s">
+        <v>101</v>
+      </c>
+      <c r="U13" s="67" t="s">
         <v>96</v>
-      </c>
-      <c r="T13" s="69" t="s">
-        <v>104</v>
-      </c>
-      <c r="U13" s="67" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4242,30 +4306,30 @@
         <v>10</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C14" s="37" t="s">
         <v>85</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="E14" s="39"/>
       <c r="F14" s="40"/>
       <c r="G14" s="41" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="H14" s="42">
         <v>12</v>
       </c>
       <c r="I14" s="43" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="J14" s="44" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="K14" s="45" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L14" s="45" t="s">
         <v>1</v>
@@ -4282,16 +4346,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="49" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="S14" s="70" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="T14" s="71" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="U14" s="70" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -4299,31 +4363,31 @@
         <v>10</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>85</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H15" s="19">
         <v>13</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="L15" s="20" t="s">
         <v>14</v>
@@ -4331,25 +4395,25 @@
       <c r="M15" s="20"/>
       <c r="N15" s="20"/>
       <c r="O15" s="21" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="P15" s="32" t="s">
         <v>3</v>
       </c>
       <c r="Q15" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="R15" s="34" t="s">
         <v>88</v>
-      </c>
-      <c r="R15" s="34" t="s">
-        <v>89</v>
       </c>
       <c r="S15" s="3" t="s">
         <v>85</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="U15" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -4357,31 +4421,31 @@
         <v>10</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>85</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="H16" s="19">
         <v>14</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>163</v>
+        <v>214</v>
       </c>
       <c r="K16" s="20" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="L16" s="20" t="s">
         <v>14</v>
@@ -4389,25 +4453,25 @@
       <c r="M16" s="20"/>
       <c r="N16" s="20"/>
       <c r="O16" s="21" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="P16" s="32" t="s">
         <v>3</v>
       </c>
       <c r="Q16" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="R16" s="34" t="s">
         <v>88</v>
-      </c>
-      <c r="R16" s="34" t="s">
-        <v>89</v>
       </c>
       <c r="S16" s="3" t="s">
         <v>85</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -4415,31 +4479,31 @@
         <v>10</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>85</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="H17" s="27">
         <v>15</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="K17" s="20" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L17" s="20" t="s">
         <v>14</v>
@@ -4455,16 +4519,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="S17" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="T17" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="U17" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="T17" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="U17" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -4472,31 +4536,31 @@
         <v>10</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>85</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>107</v>
+        <v>220</v>
       </c>
       <c r="H18" s="27">
         <v>16</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L18" s="20" t="s">
         <v>14</v>
@@ -4512,49 +4576,49 @@
         <v>6</v>
       </c>
       <c r="R18" s="34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="S18" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="T18" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="U18" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="T18" s="23" t="s">
-        <v>209</v>
-      </c>
-      <c r="U18" s="22" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:21" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="52" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="53" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C19" s="54" t="s">
         <v>85</v>
       </c>
       <c r="D19" s="55" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="E19" s="56" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="F19" s="57"/>
       <c r="G19" s="58" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="H19" s="60">
         <v>17</v>
       </c>
       <c r="I19" s="60" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J19" s="61" t="s">
-        <v>166</v>
+        <v>215</v>
       </c>
       <c r="K19" s="62" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L19" s="62" t="s">
         <v>14</v>
@@ -4571,16 +4635,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="66" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="S19" s="73" t="s">
+        <v>94</v>
+      </c>
+      <c r="T19" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="U19" s="73" t="s">
         <v>96</v>
-      </c>
-      <c r="T19" s="74" t="s">
-        <v>105</v>
-      </c>
-      <c r="U19" s="73" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4588,30 +4652,30 @@
         <v>10</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C20" s="37" t="s">
         <v>85</v>
       </c>
       <c r="D20" s="77" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="E20" s="39"/>
       <c r="F20" s="40"/>
       <c r="G20" s="41" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="H20" s="42">
         <v>18</v>
       </c>
       <c r="I20" s="43" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J20" s="44" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="K20" s="45" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="L20" s="45" t="s">
         <v>14</v>
@@ -4619,25 +4683,25 @@
       <c r="M20" s="45"/>
       <c r="N20" s="45"/>
       <c r="O20" s="46" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="P20" s="47" t="s">
         <v>3</v>
       </c>
       <c r="Q20" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="R20" s="49" t="s">
         <v>88</v>
-      </c>
-      <c r="R20" s="49" t="s">
-        <v>89</v>
       </c>
       <c r="S20" s="70" t="s">
         <v>85</v>
       </c>
       <c r="T20" s="72" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="U20" s="70" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -4645,28 +4709,31 @@
         <v>10</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>85</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>221</v>
+        <v>201</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>217</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="H21" s="27">
         <v>19</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>171</v>
+        <v>216</v>
       </c>
       <c r="K21" s="20" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="L21" s="20" t="s">
         <v>14</v>
@@ -4674,25 +4741,25 @@
       <c r="M21" s="20"/>
       <c r="N21" s="20"/>
       <c r="O21" s="21" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="P21" s="32" t="s">
         <v>3</v>
       </c>
       <c r="Q21" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="R21" s="34" t="s">
         <v>88</v>
-      </c>
-      <c r="R21" s="34" t="s">
-        <v>89</v>
       </c>
       <c r="S21" s="3" t="s">
         <v>85</v>
       </c>
       <c r="T21" s="4" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="U21" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4700,32 +4767,32 @@
         <v>10</v>
       </c>
       <c r="B22" s="53" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C22" s="54" t="s">
         <v>85</v>
       </c>
       <c r="D22" s="78" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="E22" s="56" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="F22" s="57"/>
       <c r="G22" s="58" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="H22" s="60">
         <v>20</v>
       </c>
       <c r="I22" s="60" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J22" s="68" t="s">
-        <v>174</v>
+        <v>218</v>
       </c>
       <c r="K22" s="62" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="L22" s="62" t="s">
         <v>14</v>
@@ -4733,7 +4800,7 @@
       <c r="M22" s="62"/>
       <c r="N22" s="62"/>
       <c r="O22" s="63" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="P22" s="64" t="s">
         <v>3</v>
@@ -4742,16 +4809,16 @@
         <v>8</v>
       </c>
       <c r="R22" s="66" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="S22" s="73" t="s">
         <v>85</v>
       </c>
       <c r="T22" s="74" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="U22" s="73" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4759,30 +4826,30 @@
         <v>10</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C23" s="37" t="s">
         <v>85</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E23" s="39"/>
       <c r="F23" s="40"/>
       <c r="G23" s="41" t="s">
-        <v>176</v>
+        <v>223</v>
       </c>
       <c r="H23" s="42">
         <v>21</v>
       </c>
       <c r="I23" s="43" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J23" s="75" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="K23" s="45" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="L23" s="45" t="s">
         <v>14</v>
@@ -4790,25 +4857,25 @@
       <c r="M23" s="45"/>
       <c r="N23" s="45"/>
       <c r="O23" s="46" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="P23" s="47" t="s">
         <v>3</v>
       </c>
       <c r="Q23" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="R23" s="49" t="s">
         <v>88</v>
-      </c>
-      <c r="R23" s="49" t="s">
-        <v>89</v>
       </c>
       <c r="S23" s="70" t="s">
         <v>85</v>
       </c>
       <c r="T23" s="72" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="U23" s="70" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4816,30 +4883,30 @@
         <v>10</v>
       </c>
       <c r="B24" s="53" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C24" s="54" t="s">
         <v>85</v>
       </c>
       <c r="D24" s="55" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E24" s="56"/>
       <c r="F24" s="57"/>
       <c r="G24" s="58" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="H24" s="59">
         <v>22</v>
       </c>
       <c r="I24" s="60" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="J24" s="68" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="K24" s="62" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L24" s="62" t="s">
         <v>16</v>
@@ -4856,49 +4923,49 @@
         <v>6</v>
       </c>
       <c r="R24" s="66" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="S24" s="73" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="T24" s="74" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="U24" s="73" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A25" s="35" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C25" s="37" t="s">
         <v>85</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="E25" s="39" t="s">
         <v>18</v>
       </c>
       <c r="F25" s="40"/>
       <c r="G25" s="76" t="s">
-        <v>181</v>
+        <v>18</v>
       </c>
       <c r="H25" s="43">
         <v>23</v>
       </c>
       <c r="I25" s="43" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J25" s="75" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="K25" s="45" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L25" s="45" t="s">
         <v>18</v>
@@ -4920,31 +4987,31 @@
         <v>10</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>85</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H26" s="27">
         <v>24</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="K26" s="20" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L26" s="20" t="s">
         <v>14</v>
@@ -4960,48 +5027,48 @@
         <v>6</v>
       </c>
       <c r="R26" s="34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="S26" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="T26" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="U26" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="T26" s="23" t="s">
-        <v>214</v>
-      </c>
-      <c r="U26" s="22" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:21" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>85</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="H27" s="27">
         <v>25</v>
       </c>
       <c r="I27" s="19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="K27" s="20" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L27" s="20" t="s">
         <v>14</v>
@@ -5127,187 +5194,187 @@
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="30" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="30" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="30" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="30" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="30" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="30" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="30" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="30" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="30" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="30" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="30" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="30" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="30" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="30" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="30" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="30" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="30" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="30" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="30" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="30" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="30" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="30" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="30" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="30" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="30" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="30" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="30" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="30" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="30" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="30" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="30" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="30" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="30" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="30" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="30" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="30" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="30" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>